<commit_message>
worked on corner cases of reconciliation
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/PortalBTRC/Downloads/CDR_comparer_export.xlsx
+++ b/TelcobrightVS13/Projects/PortalBTRC/Downloads/CDR_comparer_export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>FileName</t>
   </si>
@@ -38,115 +38,43 @@
     <t>VCDR.20231202.012443.364236</t>
   </si>
   <si>
-    <t>11230</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>2220532.39</t>
-  </si>
-  <si>
-    <t>0.00</t>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>File Missing</t>
   </si>
   <si>
     <t>VCDR.20231202.005751.364235</t>
   </si>
   <si>
-    <t>12019</t>
-  </si>
-  <si>
-    <t>2275329.26</t>
-  </si>
-  <si>
     <t>VCDR.20231202.003645.364234</t>
   </si>
   <si>
-    <t>12541</t>
-  </si>
-  <si>
-    <t>2236051.04</t>
-  </si>
-  <si>
     <t>VCDR.20231202.002001.364233</t>
   </si>
   <si>
-    <t>13441</t>
-  </si>
-  <si>
-    <t>2426381.72</t>
-  </si>
-  <si>
     <t>VCDR.20231202.000633.364232</t>
   </si>
   <si>
-    <t>13393</t>
-  </si>
-  <si>
-    <t>2102012.01</t>
-  </si>
-  <si>
     <t>VCDR.20231201.235527.364231</t>
   </si>
   <si>
-    <t>13931</t>
-  </si>
-  <si>
-    <t>2519630.57</t>
-  </si>
-  <si>
     <t>VCDR.20231201.234541.364230</t>
   </si>
   <si>
-    <t>14325</t>
-  </si>
-  <si>
-    <t>2368217.31</t>
-  </si>
-  <si>
     <t>VCDR.20231201.233659.364229</t>
   </si>
   <si>
-    <t>14467</t>
-  </si>
-  <si>
-    <t>2462226.62</t>
-  </si>
-  <si>
     <t>VCDR.20231201.232905.364228</t>
   </si>
   <si>
-    <t>14651</t>
-  </si>
-  <si>
-    <t>2487605.43</t>
-  </si>
-  <si>
     <t>VCDR.20231201.232159.364227</t>
   </si>
   <si>
-    <t>14670</t>
-  </si>
-  <si>
-    <t>2304730.31</t>
-  </si>
-  <si>
     <t>VCDR.20231201.231525.364226</t>
   </si>
   <si>
-    <t>14911</t>
-  </si>
-  <si>
-    <t>2418165.42</t>
-  </si>
-  <si>
     <t>VCDR.20231201.230921.364225</t>
-  </si>
-  <si>
-    <t>14992</t>
-  </si>
-  <si>
-    <t>2434905.22</t>
   </si>
 </sst>
 </file>
@@ -229,272 +157,272 @@
         <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>